<commit_message>
try to fix error
</commit_message>
<xml_diff>
--- a/Backend/Data/ProductData/productData.xlsx
+++ b/Backend/Data/ProductData/productData.xlsx
@@ -28,13 +28,13 @@
     <t>Nitesh</t>
   </si>
   <si>
-    <t>milk</t>
+    <t>petrol</t>
   </si>
   <si>
     <t>2025-01-07</t>
   </si>
   <si>
-    <t>55</t>
+    <t>120</t>
   </si>
 </sst>
 </file>

</xml_diff>